<commit_message>
updated worldstats data and config
</commit_message>
<xml_diff>
--- a/DataSets/worldstats.xlsx
+++ b/DataSets/worldstats.xlsx
@@ -1,81 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adaptabletools/Code/demo/adaptableblotter-demo/DataSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUSSAR\Documents\GitHub\adaptableblotter-demo\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3857BE-F5C1-1A4A-8C22-B70441922CF2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BEE4FE-8055-460C-B80A-2A2B995ED18C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30940" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1656" yWindow="3372" windowWidth="20412" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WorldStats" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WorldStats!$A$1:$AH$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WorldStats!$A$1:$AO$25</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>Population Total</t>
-  </si>
-  <si>
-    <t>Population Growth (%)</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>GDP per Capita</t>
-  </si>
-  <si>
     <t>GDP Growth (%)</t>
   </si>
   <si>
     <t>Trade (% of GDP)</t>
   </si>
   <si>
-    <t>Debt Total</t>
-  </si>
-  <si>
     <t>Debt per GDP (%)</t>
   </si>
   <si>
     <t>Internet Users</t>
   </si>
   <si>
-    <t>Electricity Production (kWh)</t>
-  </si>
-  <si>
-    <t>Electricity Coal (kWh)</t>
-  </si>
-  <si>
-    <t>Electricity Water</t>
-  </si>
-  <si>
-    <t>Electricity Gas</t>
-  </si>
-  <si>
-    <t>Electricity Nuclear</t>
-  </si>
-  <si>
-    <t>Electricity Oil</t>
-  </si>
-  <si>
-    <t>Electricity Renewable</t>
-  </si>
-  <si>
     <t>Air Passengers</t>
   </si>
   <si>
@@ -247,15 +211,9 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Population Density</t>
-  </si>
-  <si>
     <t>Roads Density</t>
   </si>
   <si>
-    <t>Population Urban (%)</t>
-  </si>
-  <si>
     <t>Birth Rate</t>
   </si>
   <si>
@@ -283,13 +241,79 @@
     <t>Armed Forces (% labor force)</t>
   </si>
   <si>
-    <t>Debt per Capita</t>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Growth (%)</t>
+  </si>
+  <si>
+    <t>Coal %</t>
+  </si>
+  <si>
+    <t>Water %</t>
+  </si>
+  <si>
+    <t>Gas %</t>
+  </si>
+  <si>
+    <t>Nuclear %</t>
+  </si>
+  <si>
+    <t>Oil %</t>
+  </si>
+  <si>
+    <t>Renewable %</t>
+  </si>
+  <si>
+    <t>Urbanization (%)</t>
+  </si>
+  <si>
+    <t>Debt Total (T)</t>
+  </si>
+  <si>
+    <t>GDP (T)</t>
+  </si>
+  <si>
+    <t>GDP per Capita (K)</t>
+  </si>
+  <si>
+    <t>Coal (T)</t>
+  </si>
+  <si>
+    <t>Water (T)</t>
+  </si>
+  <si>
+    <t>Gas (T)</t>
+  </si>
+  <si>
+    <t>Nuclear (T)</t>
+  </si>
+  <si>
+    <t>Oil (T)</t>
+  </si>
+  <si>
+    <t>Renewable (T)</t>
+  </si>
+  <si>
+    <t>Electricity Usage (M)</t>
+  </si>
+  <si>
+    <t>Debt per Capita (K)</t>
+  </si>
+  <si>
+    <t>Electricity Production (T)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -767,9 +791,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1125,163 +1150,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M15" sqref="M15"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.77734375" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" customWidth="1"/>
+    <col min="23" max="34" width="12.77734375" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" customWidth="1"/>
+    <col min="37" max="37" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.5546875" customWidth="1"/>
+    <col min="41" max="41" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AE1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AF1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AG1" t="s">
         <v>79</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AH1" t="s">
         <v>80</v>
       </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="AI1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AK1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U1" t="s">
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
       <c r="D2">
         <v>313873685</v>
@@ -1308,10 +1351,10 @@
         <v>9150000</v>
       </c>
       <c r="L2" s="1">
-        <v>16200000000000</v>
-      </c>
-      <c r="M2">
-        <v>51755</v>
+        <v>16.2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>51.6</v>
       </c>
       <c r="N2">
         <v>2.5099999999999998</v>
@@ -1320,13 +1363,13 @@
         <v>30</v>
       </c>
       <c r="P2" s="1">
-        <v>17300000000000</v>
-      </c>
-      <c r="Q2">
-        <v>52170</v>
-      </c>
-      <c r="R2">
-        <v>106</v>
+        <v>17.3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>52.2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>106.8</v>
       </c>
       <c r="S2">
         <v>90341000</v>
@@ -1334,64 +1377,85 @@
       <c r="T2">
         <v>28.5</v>
       </c>
-      <c r="U2" s="1">
-        <v>4330000000000</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1880000000000</v>
+      <c r="U2">
+        <v>1.48</v>
+      </c>
+      <c r="V2" s="2">
+        <v>464.2</v>
       </c>
       <c r="W2" s="1">
-        <v>322000000000</v>
+        <v>188</v>
       </c>
       <c r="X2" s="1">
-        <v>1050000000000</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="Y2" s="1">
-        <v>821000000000</v>
-      </c>
-      <c r="Z2">
-        <v>39524000000</v>
+        <v>105</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>82.1</v>
       </c>
       <c r="AA2" s="1">
-        <v>529000000000</v>
-      </c>
-      <c r="AB2">
+        <v>3.95</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>52.9</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>40.5</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>6.94</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>22.62</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="AI2">
         <v>66.599999999999994</v>
       </c>
-      <c r="AC2">
+      <c r="AJ2">
         <v>737000000</v>
       </c>
-      <c r="AD2">
+      <c r="AK2">
         <v>782</v>
       </c>
-      <c r="AE2">
+      <c r="AL2">
         <v>2.9</v>
       </c>
-      <c r="AF2">
+      <c r="AM2">
         <v>91</v>
       </c>
-      <c r="AG2">
+      <c r="AN2">
         <v>0.94</v>
       </c>
-      <c r="AH2">
+      <c r="AO2">
         <v>1490000</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>1350695000</v>
       </c>
       <c r="E3">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F3">
         <v>0.48</v>
@@ -1412,10 +1476,10 @@
         <v>9330000</v>
       </c>
       <c r="L3" s="1">
-        <v>8230000000000</v>
-      </c>
-      <c r="M3">
-        <v>6093</v>
+        <v>8.23</v>
+      </c>
+      <c r="M3" s="2">
+        <v>6.1</v>
       </c>
       <c r="N3">
         <v>10.4</v>
@@ -1424,13 +1488,13 @@
         <v>52</v>
       </c>
       <c r="P3" s="1">
-        <v>3000000000000</v>
-      </c>
-      <c r="Q3">
-        <v>2221</v>
-      </c>
-      <c r="R3">
-        <v>37.5</v>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R3" s="2">
+        <v>36.5</v>
       </c>
       <c r="S3">
         <v>175183000</v>
@@ -1438,64 +1502,85 @@
       <c r="T3">
         <v>12.7</v>
       </c>
-      <c r="U3" s="1">
-        <v>4720000000000</v>
-      </c>
-      <c r="V3" s="1">
-        <v>3720000000000</v>
+      <c r="U3">
+        <v>0.4</v>
+      </c>
+      <c r="V3" s="2">
+        <v>540</v>
       </c>
       <c r="W3" s="1">
-        <v>699000000000</v>
-      </c>
-      <c r="X3">
-        <v>84022000000</v>
-      </c>
-      <c r="Y3">
-        <v>86350000000</v>
-      </c>
-      <c r="Z3">
-        <v>7857000000</v>
+        <v>372</v>
+      </c>
+      <c r="X3" s="1">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>8.64</v>
       </c>
       <c r="AA3" s="1">
-        <v>803000000000</v>
-      </c>
-      <c r="AB3">
+        <v>0.79</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>80.3</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>68.89</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>12.94</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>1.56</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>14.87</v>
+      </c>
+      <c r="AI3">
         <v>41.8</v>
       </c>
-      <c r="AC3">
+      <c r="AJ3">
         <v>318000000</v>
       </c>
-      <c r="AD3">
+      <c r="AK3">
         <v>58</v>
       </c>
-      <c r="AE3">
+      <c r="AL3">
         <v>3.8</v>
       </c>
-      <c r="AF3">
+      <c r="AM3">
         <v>63</v>
       </c>
-      <c r="AG3">
+      <c r="AN3">
         <v>0.38</v>
       </c>
-      <c r="AH3">
+      <c r="AO3">
         <v>2990000</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>127561489</v>
       </c>
       <c r="E4">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F4">
         <v>-0.08</v>
@@ -1516,10 +1601,10 @@
         <v>365000</v>
       </c>
       <c r="L4" s="1">
-        <v>5940000000000</v>
-      </c>
-      <c r="M4">
-        <v>46548</v>
+        <v>5.94</v>
+      </c>
+      <c r="M4" s="2">
+        <v>46.6</v>
       </c>
       <c r="N4">
         <v>4.6500000000000004</v>
@@ -1528,13 +1613,13 @@
         <v>31</v>
       </c>
       <c r="P4" s="1">
-        <v>3020000000000</v>
-      </c>
-      <c r="Q4">
-        <v>24000</v>
-      </c>
-      <c r="R4">
-        <v>60</v>
+        <v>3.02</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>24</v>
+      </c>
+      <c r="R4" s="2">
+        <v>50.8</v>
       </c>
       <c r="S4">
         <v>36108452</v>
@@ -1542,64 +1627,85 @@
       <c r="T4">
         <v>28.4</v>
       </c>
-      <c r="U4" s="1">
-        <v>1040000000000</v>
-      </c>
-      <c r="V4" s="1">
-        <v>281000000000</v>
-      </c>
-      <c r="W4">
-        <v>83197000000</v>
+      <c r="U4">
+        <v>0.84</v>
+      </c>
+      <c r="V4" s="2">
+        <v>107.2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>28.1</v>
       </c>
       <c r="X4" s="1">
-        <v>374000000000</v>
+        <v>8.32</v>
       </c>
       <c r="Y4" s="1">
-        <v>102000000000</v>
+        <v>37.4</v>
       </c>
       <c r="Z4" s="1">
-        <v>105000000000</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AA4" s="1">
-        <v>127000000000</v>
-      </c>
-      <c r="AB4">
+        <v>10.5</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>26.21</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>7.76</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>34.880000000000003</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>9.51</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>11.84</v>
+      </c>
+      <c r="AI4">
         <v>89.1</v>
       </c>
-      <c r="AC4">
+      <c r="AJ4">
         <v>98900000</v>
       </c>
-      <c r="AD4">
+      <c r="AK4">
         <v>590</v>
       </c>
-      <c r="AE4">
+      <c r="AL4">
         <v>2.5</v>
       </c>
-      <c r="AF4">
+      <c r="AM4">
         <v>97</v>
       </c>
-      <c r="AG4">
+      <c r="AN4">
         <v>0.4</v>
       </c>
-      <c r="AH4">
+      <c r="AO4">
         <v>260000</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>80425823</v>
       </c>
       <c r="E5">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F5">
         <v>-0.15</v>
@@ -1620,10 +1726,10 @@
         <v>349000</v>
       </c>
       <c r="L5" s="1">
-        <v>3430000000000</v>
-      </c>
-      <c r="M5">
-        <v>42598</v>
+        <v>3.43</v>
+      </c>
+      <c r="M5" s="2">
+        <v>42.6</v>
       </c>
       <c r="N5">
         <v>4.01</v>
@@ -1632,13 +1738,13 @@
         <v>98</v>
       </c>
       <c r="P5" s="1">
-        <v>5720000000000</v>
-      </c>
-      <c r="Q5">
-        <v>57755</v>
-      </c>
-      <c r="R5">
-        <v>142</v>
+        <v>5.72</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>57.8</v>
+      </c>
+      <c r="R5" s="2">
+        <v>166.8</v>
       </c>
       <c r="S5">
         <v>27906896</v>
@@ -1646,64 +1752,85 @@
       <c r="T5">
         <v>33.700000000000003</v>
       </c>
-      <c r="U5" s="1">
-        <v>602000000000</v>
-      </c>
-      <c r="V5" s="1">
-        <v>272000000000</v>
-      </c>
-      <c r="W5">
-        <v>17268000000</v>
-      </c>
-      <c r="X5">
-        <v>83630000000</v>
+      <c r="U5">
+        <v>0.76</v>
+      </c>
+      <c r="V5" s="2">
+        <v>61.1</v>
+      </c>
+      <c r="W5" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1.73</v>
       </c>
       <c r="Y5" s="1">
-        <v>108000000000</v>
-      </c>
-      <c r="Z5">
-        <v>6608000000</v>
+        <v>8.36</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>10.8</v>
       </c>
       <c r="AA5" s="1">
-        <v>123000000000</v>
-      </c>
-      <c r="AB5">
+        <v>0.66</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>44.55</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2.83</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>13.7</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>20.149999999999999</v>
+      </c>
+      <c r="AI5">
         <v>180</v>
       </c>
-      <c r="AC5">
+      <c r="AJ5">
         <v>106000000</v>
       </c>
-      <c r="AD5">
+      <c r="AK5">
         <v>572</v>
       </c>
-      <c r="AE5">
+      <c r="AL5">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AF5">
+      <c r="AM5">
         <v>106</v>
       </c>
-      <c r="AG5">
+      <c r="AN5">
         <v>0.45</v>
       </c>
-      <c r="AH5">
+      <c r="AO5">
         <v>186000</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>65676758</v>
       </c>
       <c r="E6">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F6">
         <v>0.49</v>
@@ -1724,10 +1851,10 @@
         <v>548000</v>
       </c>
       <c r="L6" s="1">
-        <v>2610000000000</v>
-      </c>
-      <c r="M6">
-        <v>39759</v>
+        <v>2.61</v>
+      </c>
+      <c r="M6" s="2">
+        <v>39.700000000000003</v>
       </c>
       <c r="N6">
         <v>1.72</v>
@@ -1736,13 +1863,13 @@
         <v>57</v>
       </c>
       <c r="P6" s="1">
-        <v>5280000000000</v>
-      </c>
-      <c r="Q6">
-        <v>74619</v>
-      </c>
-      <c r="R6">
-        <v>182</v>
+        <v>5.28</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="R6" s="2">
+        <v>202.3</v>
       </c>
       <c r="S6">
         <v>23975000</v>
@@ -1750,64 +1877,85 @@
       <c r="T6">
         <v>37.5</v>
       </c>
-      <c r="U6" s="1">
-        <v>557000000000</v>
-      </c>
-      <c r="V6">
-        <v>17310000000</v>
-      </c>
-      <c r="W6">
-        <v>44819000000</v>
-      </c>
-      <c r="X6">
-        <v>26755000000</v>
+      <c r="U6">
+        <v>0.78</v>
+      </c>
+      <c r="V6" s="2">
+        <v>50.9</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1.73</v>
+      </c>
+      <c r="X6" s="1">
+        <v>4.4800000000000004</v>
       </c>
       <c r="Y6" s="1">
-        <v>352000000000</v>
-      </c>
-      <c r="Z6">
-        <v>3439000000</v>
-      </c>
-      <c r="AA6">
-        <v>64789000000</v>
-      </c>
-      <c r="AB6">
+        <v>2.68</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>6.48</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>5.26</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>69.14</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>12.73</v>
+      </c>
+      <c r="AI6">
         <v>191</v>
       </c>
-      <c r="AC6">
+      <c r="AJ6">
         <v>64700000</v>
       </c>
-      <c r="AD6">
+      <c r="AK6">
         <v>580</v>
       </c>
-      <c r="AE6">
+      <c r="AL6">
         <v>6.4</v>
       </c>
-      <c r="AF6">
+      <c r="AM6">
         <v>91</v>
       </c>
-      <c r="AG6">
+      <c r="AN6">
         <v>1.08</v>
       </c>
-      <c r="AH6">
+      <c r="AO6">
         <v>326000</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>63695687</v>
       </c>
       <c r="E7">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="F7">
         <v>0.78</v>
@@ -1828,10 +1976,10 @@
         <v>242000</v>
       </c>
       <c r="L7" s="1">
-        <v>2460000000000</v>
-      </c>
-      <c r="M7">
-        <v>38649</v>
+        <v>2.46</v>
+      </c>
+      <c r="M7" s="2">
+        <v>38.6</v>
       </c>
       <c r="N7">
         <v>1.66</v>
@@ -1840,13 +1988,13 @@
         <v>66</v>
       </c>
       <c r="P7" s="1">
-        <v>10100000000000</v>
-      </c>
-      <c r="Q7">
-        <v>160158</v>
-      </c>
-      <c r="R7">
-        <v>406</v>
+        <v>10.1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>160.19999999999999</v>
+      </c>
+      <c r="R7" s="2">
+        <v>410.6</v>
       </c>
       <c r="S7">
         <v>21618675</v>
@@ -1854,58 +2002,79 @@
       <c r="T7">
         <v>34.4</v>
       </c>
-      <c r="U7" s="1">
-        <v>365000000000</v>
-      </c>
-      <c r="V7" s="1">
-        <v>110000000000</v>
-      </c>
-      <c r="W7">
-        <v>5686000000</v>
+      <c r="U7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="V7" s="2">
+        <v>37</v>
+      </c>
+      <c r="W7" s="1">
+        <v>11</v>
       </c>
       <c r="X7" s="1">
-        <v>147000000000</v>
-      </c>
-      <c r="Y7">
-        <v>68980000000</v>
-      </c>
-      <c r="Z7">
-        <v>3665000000</v>
-      </c>
-      <c r="AA7">
-        <v>34408000000</v>
-      </c>
-      <c r="AB7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>3.44</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>29.75</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>39.76</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>18.66</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>9.31</v>
+      </c>
+      <c r="AI7">
         <v>172</v>
       </c>
-      <c r="AC7">
+      <c r="AJ7">
         <v>115000000</v>
       </c>
-      <c r="AD7">
+      <c r="AK7">
         <v>518</v>
       </c>
-      <c r="AE7">
+      <c r="AL7">
         <v>2.9</v>
       </c>
-      <c r="AF7">
+      <c r="AM7">
         <v>124</v>
       </c>
-      <c r="AG7">
+      <c r="AN7">
         <v>0.52</v>
       </c>
-      <c r="AH7">
+      <c r="AO7">
         <v>169000</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>198656019</v>
@@ -1932,10 +2101,10 @@
         <v>8460000</v>
       </c>
       <c r="L8" s="1">
-        <v>2250000000000</v>
-      </c>
-      <c r="M8">
-        <v>11320</v>
+        <v>2.25</v>
+      </c>
+      <c r="M8" s="2">
+        <v>11.3</v>
       </c>
       <c r="N8">
         <v>7.53</v>
@@ -1944,13 +2113,13 @@
         <v>27</v>
       </c>
       <c r="P8" s="1">
-        <v>428000000000</v>
-      </c>
-      <c r="Q8">
-        <v>1608</v>
-      </c>
-      <c r="R8">
-        <v>15</v>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="R8" s="2">
+        <v>19</v>
       </c>
       <c r="S8">
         <v>18186476</v>
@@ -1958,58 +2127,79 @@
       <c r="T8">
         <v>9.15</v>
       </c>
-      <c r="U8" s="1">
-        <v>532000000000</v>
-      </c>
-      <c r="V8">
-        <v>12379000000</v>
+      <c r="U8">
+        <v>0.48</v>
+      </c>
+      <c r="V8" s="2">
+        <v>95.9</v>
       </c>
       <c r="W8" s="1">
-        <v>428000000000</v>
-      </c>
-      <c r="X8">
-        <v>25095000000</v>
-      </c>
-      <c r="Y8">
-        <v>15659000000</v>
-      </c>
-      <c r="Z8">
-        <v>14796000000</v>
+        <v>1.24</v>
+      </c>
+      <c r="X8" s="1">
+        <v>42.8</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>1.57</v>
       </c>
       <c r="AA8" s="1">
-        <v>463000000000</v>
-      </c>
-      <c r="AB8">
+        <v>1.48</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>46.3</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>44.63</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>1.63</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>48.28</v>
+      </c>
+      <c r="AI8">
         <v>18.600000000000001</v>
       </c>
-      <c r="AC8">
+      <c r="AJ8">
         <v>94800000</v>
       </c>
-      <c r="AD8">
+      <c r="AK8">
         <v>244</v>
       </c>
-      <c r="AE8">
+      <c r="AL8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="AF8">
+      <c r="AM8">
         <v>101</v>
       </c>
-      <c r="AG8">
+      <c r="AN8">
         <v>0.68</v>
       </c>
-      <c r="AH8">
+      <c r="AO8">
         <v>713000</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>143178000</v>
@@ -2036,10 +2226,10 @@
         <v>16400000</v>
       </c>
       <c r="L9" s="1">
-        <v>2020000000000</v>
-      </c>
-      <c r="M9">
-        <v>14091</v>
+        <v>2.02</v>
+      </c>
+      <c r="M9" s="2">
+        <v>14.1</v>
       </c>
       <c r="N9">
         <v>4.5</v>
@@ -2048,13 +2238,13 @@
         <v>52</v>
       </c>
       <c r="P9" s="1">
-        <v>632000000000</v>
-      </c>
-      <c r="Q9">
-        <v>3634</v>
-      </c>
-      <c r="R9">
-        <v>23</v>
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="R9" s="2">
+        <v>31.3</v>
       </c>
       <c r="S9">
         <v>20703653</v>
@@ -2062,64 +2252,85 @@
       <c r="T9">
         <v>14.5</v>
       </c>
-      <c r="U9" s="1">
-        <v>1050000000000</v>
-      </c>
-      <c r="V9" s="1">
-        <v>164000000000</v>
+      <c r="U9">
+        <v>0.85</v>
+      </c>
+      <c r="V9" s="2">
+        <v>121.5</v>
       </c>
       <c r="W9" s="1">
-        <v>166000000000</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="X9" s="1">
-        <v>519000000000</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="Y9" s="1">
-        <v>173000000000</v>
-      </c>
-      <c r="Z9">
-        <v>27345000000</v>
+        <v>51.9</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>17.3</v>
       </c>
       <c r="AA9" s="1">
-        <v>166000000000</v>
-      </c>
-      <c r="AB9">
+        <v>2.73</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>13.49</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>13.66</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>42.7</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>14.23</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>13.66</v>
+      </c>
+      <c r="AI9">
         <v>5.87</v>
       </c>
-      <c r="AC9">
+      <c r="AJ9">
         <v>58700000</v>
       </c>
-      <c r="AD9">
+      <c r="AK9">
         <v>131</v>
       </c>
-      <c r="AE9">
+      <c r="AL9">
         <v>2.4</v>
       </c>
-      <c r="AF9">
+      <c r="AM9">
         <v>166</v>
       </c>
-      <c r="AG9">
+      <c r="AN9">
         <v>1.77</v>
       </c>
-      <c r="AH9">
+      <c r="AO9">
         <v>1360000</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>59539717</v>
       </c>
       <c r="E10">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F10">
         <v>0.31</v>
@@ -2140,10 +2351,10 @@
         <v>294000</v>
       </c>
       <c r="L10" s="1">
-        <v>2010000000000</v>
-      </c>
-      <c r="M10">
-        <v>33814</v>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="M10" s="2">
+        <v>33.799999999999997</v>
       </c>
       <c r="N10">
         <v>1.72</v>
@@ -2152,13 +2363,13 @@
         <v>59</v>
       </c>
       <c r="P10" s="1">
-        <v>2460000000000</v>
-      </c>
-      <c r="Q10">
-        <v>36841</v>
-      </c>
-      <c r="R10">
-        <v>108</v>
+        <v>2.46</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="R10" s="2">
+        <v>122.4</v>
       </c>
       <c r="S10">
         <v>13483000</v>
@@ -2166,64 +2377,85 @@
       <c r="T10">
         <v>22.1</v>
       </c>
-      <c r="U10" s="1">
-        <v>301000000000</v>
-      </c>
-      <c r="V10">
-        <v>50139000000</v>
-      </c>
-      <c r="W10">
-        <v>45823000000</v>
+      <c r="U10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="V10" s="2">
+        <v>34.4</v>
+      </c>
+      <c r="W10" s="1">
+        <v>5.01</v>
       </c>
       <c r="X10" s="1">
-        <v>145000000000</v>
+        <v>4.58</v>
       </c>
       <c r="Y10" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="Z10" s="1">
         <v>0</v>
       </c>
-      <c r="Z10">
-        <v>19885000000</v>
-      </c>
-      <c r="AA10">
-        <v>82962000000</v>
-      </c>
-      <c r="AB10">
+      <c r="AA10" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>14.58</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>13.33</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>42.17</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>5.78</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>24.13</v>
+      </c>
+      <c r="AI10">
         <v>131</v>
       </c>
-      <c r="AC10">
+      <c r="AJ10">
         <v>31100000</v>
       </c>
-      <c r="AD10">
+      <c r="AK10">
         <v>679</v>
       </c>
-      <c r="AE10">
+      <c r="AL10">
         <v>3.4</v>
       </c>
-      <c r="AF10">
+      <c r="AM10">
         <v>155</v>
       </c>
-      <c r="AG10">
+      <c r="AN10">
         <v>1.43</v>
       </c>
-      <c r="AH10">
+      <c r="AO10">
         <v>360000</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>1236686732</v>
       </c>
       <c r="E11">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="F11">
         <v>1.29</v>
@@ -2244,10 +2476,10 @@
         <v>2970000</v>
       </c>
       <c r="L11" s="1">
-        <v>1860000000000</v>
-      </c>
-      <c r="M11">
-        <v>1503</v>
+        <v>1.86</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.5</v>
       </c>
       <c r="N11">
         <v>10.3</v>
@@ -2256,13 +2488,13 @@
         <v>55</v>
       </c>
       <c r="P11" s="1">
-        <v>376000000000</v>
-      </c>
-      <c r="Q11">
-        <v>240</v>
-      </c>
-      <c r="R11">
-        <v>20</v>
+        <v>0.376</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="R11" s="2">
+        <v>20.2</v>
       </c>
       <c r="S11">
         <v>14980000</v>
@@ -2270,58 +2502,79 @@
       <c r="T11">
         <v>1.21</v>
       </c>
-      <c r="U11" s="1">
-        <v>1050000000000</v>
-      </c>
-      <c r="V11" s="1">
-        <v>715000000000</v>
+      <c r="U11">
+        <v>0.1</v>
+      </c>
+      <c r="V11" s="2">
+        <v>118.4</v>
       </c>
       <c r="W11" s="1">
-        <v>131000000000</v>
+        <v>71.5</v>
       </c>
       <c r="X11" s="1">
-        <v>109000000000</v>
-      </c>
-      <c r="Y11">
-        <v>33286000000</v>
-      </c>
-      <c r="Z11">
-        <v>12223000000</v>
+        <v>13.1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>3.33</v>
       </c>
       <c r="AA11" s="1">
-        <v>183000000000</v>
-      </c>
-      <c r="AB11">
+        <v>1.22</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>60.41</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>11.07</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2.81</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>1.03</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>15.46</v>
+      </c>
+      <c r="AI11">
         <v>139</v>
       </c>
-      <c r="AC11">
+      <c r="AJ11">
         <v>72200000</v>
       </c>
-      <c r="AD11">
+      <c r="AK11">
         <v>213</v>
       </c>
-      <c r="AE11">
+      <c r="AL11">
         <v>0.7</v>
       </c>
-      <c r="AF11">
+      <c r="AM11">
         <v>62</v>
       </c>
-      <c r="AG11">
+      <c r="AN11">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AH11">
+      <c r="AO11">
         <v>2730000</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>34754312</v>
@@ -2348,10 +2601,10 @@
         <v>9090000</v>
       </c>
       <c r="L12" s="1">
-        <v>1820000000000</v>
-      </c>
-      <c r="M12">
-        <v>52409</v>
+        <v>1.82</v>
+      </c>
+      <c r="M12" s="2">
+        <v>52.4</v>
       </c>
       <c r="N12">
         <v>3.37</v>
@@ -2360,13 +2613,13 @@
         <v>62</v>
       </c>
       <c r="P12" s="1">
-        <v>1330000000000</v>
-      </c>
-      <c r="Q12">
-        <v>29625</v>
-      </c>
-      <c r="R12">
-        <v>64</v>
+        <v>1.33</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="R12" s="2">
+        <v>73.099999999999994</v>
       </c>
       <c r="S12">
         <v>11314190</v>
@@ -2374,58 +2627,79 @@
       <c r="T12">
         <v>32.5</v>
       </c>
-      <c r="U12" s="1">
-        <v>637000000000</v>
-      </c>
-      <c r="V12">
-        <v>76364000000</v>
+      <c r="U12">
+        <v>2.91</v>
+      </c>
+      <c r="V12" s="2">
+        <v>101.2</v>
       </c>
       <c r="W12" s="1">
-        <v>376000000000</v>
-      </c>
-      <c r="X12">
-        <v>62111000000</v>
-      </c>
-      <c r="Y12">
-        <v>93589000000</v>
-      </c>
-      <c r="Z12">
-        <v>6531000000</v>
+        <v>7.64</v>
+      </c>
+      <c r="X12" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>6.21</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>9.36</v>
       </c>
       <c r="AA12" s="1">
-        <v>397000000000</v>
-      </c>
-      <c r="AB12">
+        <v>0.65</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>37.17</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>6.14</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>39.24</v>
+      </c>
+      <c r="AI12">
         <v>12</v>
       </c>
-      <c r="AC12">
+      <c r="AJ12">
         <v>70500000</v>
       </c>
-      <c r="AD12">
+      <c r="AK12">
         <v>123</v>
       </c>
-      <c r="AE12">
+      <c r="AL12">
         <v>6.3</v>
       </c>
-      <c r="AF12">
+      <c r="AM12">
         <v>76</v>
       </c>
-      <c r="AG12">
+      <c r="AN12">
         <v>0.34</v>
       </c>
-      <c r="AH12">
+      <c r="AO12">
         <v>66000</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>22723900</v>
@@ -2452,10 +2726,10 @@
         <v>7680000</v>
       </c>
       <c r="L13" s="1">
-        <v>1530000000000</v>
-      </c>
-      <c r="M13">
-        <v>67436</v>
+        <v>1.53</v>
+      </c>
+      <c r="M13" s="2">
+        <v>67.3</v>
       </c>
       <c r="N13">
         <v>1.96</v>
@@ -2464,13 +2738,13 @@
         <v>43</v>
       </c>
       <c r="P13" s="1">
-        <v>1510000000000</v>
-      </c>
-      <c r="Q13">
-        <v>52596</v>
-      </c>
-      <c r="R13">
-        <v>95</v>
+        <v>1.51</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="R13" s="2">
+        <v>98.7</v>
       </c>
       <c r="S13">
         <v>5611000</v>
@@ -2478,64 +2752,85 @@
       <c r="T13">
         <v>24.3</v>
       </c>
-      <c r="U13" s="1">
-        <v>253000000000</v>
-      </c>
-      <c r="V13" s="1">
-        <v>173000000000</v>
-      </c>
-      <c r="W13">
-        <v>16756000000</v>
-      </c>
-      <c r="X13">
-        <v>49658000000</v>
-      </c>
-      <c r="Y13">
+      <c r="U13">
+        <v>1.18</v>
+      </c>
+      <c r="V13" s="2">
+        <v>26.9</v>
+      </c>
+      <c r="W13" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="X13" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>4.97</v>
+      </c>
+      <c r="Z13" s="1">
         <v>0</v>
       </c>
-      <c r="Z13">
-        <v>4103000000</v>
-      </c>
-      <c r="AA13">
-        <v>25520000000</v>
-      </c>
-      <c r="AB13">
+      <c r="AA13" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>64.3</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>6.23</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>18.46</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>1.53</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>9.49</v>
+      </c>
+      <c r="AI13">
         <v>10.7</v>
       </c>
-      <c r="AC13">
+      <c r="AJ13">
         <v>66400000</v>
       </c>
-      <c r="AD13">
+      <c r="AK13">
         <v>698</v>
       </c>
-      <c r="AE13">
+      <c r="AL13">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AF13">
+      <c r="AM13">
         <v>100</v>
       </c>
-      <c r="AG13">
+      <c r="AN13">
         <v>0.47</v>
       </c>
-      <c r="AH13">
+      <c r="AO13">
         <v>56200</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>46761264</v>
       </c>
       <c r="E14">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F14">
         <v>0.46</v>
@@ -2556,10 +2851,10 @@
         <v>499000</v>
       </c>
       <c r="L14" s="1">
-        <v>1320000000000</v>
-      </c>
-      <c r="M14">
-        <v>28282</v>
+        <v>1.32</v>
+      </c>
+      <c r="M14" s="2">
+        <v>28.2</v>
       </c>
       <c r="N14">
         <v>-0.2</v>
@@ -2568,13 +2863,13 @@
         <v>65</v>
       </c>
       <c r="P14" s="1">
-        <v>2290000000000</v>
-      </c>
-      <c r="Q14">
-        <v>52045</v>
-      </c>
-      <c r="R14">
-        <v>167</v>
+        <v>2.29</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>52</v>
+      </c>
+      <c r="R14" s="2">
+        <v>173.5</v>
       </c>
       <c r="S14">
         <v>11396347</v>
@@ -2582,64 +2877,85 @@
       <c r="T14">
         <v>24.4</v>
       </c>
-      <c r="U14" s="1">
-        <v>289000000000</v>
-      </c>
-      <c r="V14">
-        <v>44927000000</v>
-      </c>
-      <c r="W14">
-        <v>30596000000</v>
-      </c>
-      <c r="X14">
-        <v>84517000000</v>
-      </c>
-      <c r="Y14">
-        <v>57731000000</v>
-      </c>
-      <c r="Z14">
-        <v>14772000000</v>
-      </c>
-      <c r="AA14">
-        <v>86224000000</v>
-      </c>
-      <c r="AB14">
+      <c r="U14">
+        <v>0.68</v>
+      </c>
+      <c r="V14" s="2">
+        <v>31.9</v>
+      </c>
+      <c r="W14" s="1">
+        <v>4.49</v>
+      </c>
+      <c r="X14" s="1">
+        <v>3.06</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>5.77</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>1.48</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>14.09</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="AE14" s="1">
+        <v>26.51</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>18.11</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>4.63</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>27.05</v>
+      </c>
+      <c r="AI14">
         <v>132</v>
       </c>
-      <c r="AC14">
+      <c r="AJ14">
         <v>48100000</v>
       </c>
-      <c r="AD14">
+      <c r="AK14">
         <v>593</v>
       </c>
-      <c r="AE14">
+      <c r="AL14">
         <v>3.1</v>
       </c>
-      <c r="AF14">
+      <c r="AM14">
         <v>111</v>
       </c>
-      <c r="AG14">
+      <c r="AN14">
         <v>0.92</v>
       </c>
-      <c r="AH14">
+      <c r="AO14">
         <v>216000</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>50004441</v>
       </c>
       <c r="E15">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="F15">
         <v>0.46</v>
@@ -2660,10 +2976,10 @@
         <v>97100</v>
       </c>
       <c r="L15" s="1">
-        <v>1220000000000</v>
-      </c>
-      <c r="M15">
-        <v>24454</v>
+        <v>1.22</v>
+      </c>
+      <c r="M15" s="2">
+        <v>24.4</v>
       </c>
       <c r="N15">
         <v>6.5</v>
@@ -2672,13 +2988,13 @@
         <v>110</v>
       </c>
       <c r="P15" s="1">
-        <v>437000000000</v>
-      </c>
-      <c r="Q15">
-        <v>7567</v>
-      </c>
-      <c r="R15">
-        <v>37</v>
+        <v>0.437</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="R15" s="2">
+        <v>35.799999999999997</v>
       </c>
       <c r="S15">
         <v>18252201</v>
@@ -2686,64 +3002,85 @@
       <c r="T15">
         <v>37.200000000000003</v>
       </c>
-      <c r="U15" s="1">
-        <v>520000000000</v>
-      </c>
-      <c r="V15" s="1">
-        <v>225000000000</v>
-      </c>
-      <c r="W15">
-        <v>4598000000</v>
+      <c r="U15">
+        <v>1.05</v>
+      </c>
+      <c r="V15" s="2">
+        <v>52.5</v>
+      </c>
+      <c r="W15" s="1">
+        <v>22.5</v>
       </c>
       <c r="X15" s="1">
-        <v>116000000000</v>
+        <v>0.46</v>
       </c>
       <c r="Y15" s="1">
-        <v>155000000000</v>
-      </c>
-      <c r="Z15">
-        <v>16631000000</v>
-      </c>
-      <c r="AA15">
-        <v>7479000000</v>
-      </c>
-      <c r="AB15">
+        <v>11.6</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>42.88</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="AE15" s="1">
+        <v>22.11</v>
+      </c>
+      <c r="AF15" s="1">
+        <v>29.54</v>
+      </c>
+      <c r="AG15" s="1">
+        <v>3.17</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>1.43</v>
+      </c>
+      <c r="AI15">
         <v>106</v>
       </c>
-      <c r="AC15">
+      <c r="AJ15">
         <v>40000000</v>
       </c>
-      <c r="AD15">
+      <c r="AK15">
         <v>363</v>
       </c>
-      <c r="AE15">
+      <c r="AL15">
         <v>5.3</v>
       </c>
-      <c r="AF15">
+      <c r="AM15">
         <v>105</v>
       </c>
-      <c r="AG15">
+      <c r="AN15">
         <v>2.56</v>
       </c>
-      <c r="AH15">
+      <c r="AO15">
         <v>660000</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>120847477</v>
       </c>
       <c r="E16">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F16">
         <v>1.25</v>
@@ -2764,10 +3101,10 @@
         <v>1940000</v>
       </c>
       <c r="L16" s="1">
-        <v>1190000000000</v>
-      </c>
-      <c r="M16">
-        <v>9818</v>
+        <v>1.19</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9.8000000000000007</v>
       </c>
       <c r="N16">
         <v>5.1100000000000003</v>
@@ -2776,13 +3113,13 @@
         <v>66</v>
       </c>
       <c r="P16" s="1">
-        <v>353000000000</v>
-      </c>
-      <c r="Q16">
-        <v>1956</v>
-      </c>
-      <c r="R16">
-        <v>20</v>
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2</v>
+      </c>
+      <c r="R16" s="2">
+        <v>29.7</v>
       </c>
       <c r="S16">
         <v>12717139</v>
@@ -2790,64 +3127,85 @@
       <c r="T16">
         <v>10.5</v>
       </c>
-      <c r="U16" s="1">
-        <v>296000000000</v>
-      </c>
-      <c r="V16">
-        <v>34132000000</v>
-      </c>
-      <c r="W16">
-        <v>36266000000</v>
+      <c r="U16">
+        <v>0.27</v>
+      </c>
+      <c r="V16" s="2">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="W16" s="1">
+        <v>3.41</v>
       </c>
       <c r="X16" s="1">
-        <v>156000000000</v>
-      </c>
-      <c r="Y16">
-        <v>10089000000</v>
-      </c>
-      <c r="Z16">
-        <v>48371000000</v>
-      </c>
-      <c r="AA16">
-        <v>46964000000</v>
-      </c>
-      <c r="AB16">
+        <v>3.63</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>4.84</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>10.29</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>10.93</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>47.01</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>3.04</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>14.58</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="AI16">
         <v>18.899999999999999</v>
       </c>
-      <c r="AC16">
+      <c r="AJ16">
         <v>32900000</v>
       </c>
-      <c r="AD16">
+      <c r="AK16">
         <v>269</v>
       </c>
-      <c r="AE16">
+      <c r="AL16">
         <v>1.5</v>
       </c>
-      <c r="AF16">
+      <c r="AM16">
         <v>78</v>
       </c>
-      <c r="AG16">
+      <c r="AN16">
         <v>0.62</v>
       </c>
-      <c r="AH16">
+      <c r="AO16">
         <v>330000</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>73997128</v>
       </c>
       <c r="E17">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F17">
         <v>1.25</v>
@@ -2868,10 +3226,10 @@
         <v>770000</v>
       </c>
       <c r="L17" s="1">
-        <v>789000000000</v>
-      </c>
-      <c r="M17">
-        <v>10661</v>
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="M17" s="2">
+        <v>10.7</v>
       </c>
       <c r="N17">
         <v>9.16</v>
@@ -2880,13 +3238,13 @@
         <v>58</v>
       </c>
       <c r="P17" s="1">
-        <v>331000000000</v>
-      </c>
-      <c r="Q17">
-        <v>3794</v>
-      </c>
-      <c r="R17">
-        <v>40</v>
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="R17" s="2">
+        <v>42</v>
       </c>
       <c r="S17">
         <v>7858170</v>
@@ -2894,64 +3252,85 @@
       <c r="T17">
         <v>10.6</v>
       </c>
-      <c r="U17" s="1">
-        <v>229000000000</v>
-      </c>
-      <c r="V17">
-        <v>66217000000</v>
-      </c>
-      <c r="W17">
-        <v>52338000000</v>
+      <c r="U17">
+        <v>0.38</v>
+      </c>
+      <c r="V17" s="2">
+        <v>28.2</v>
+      </c>
+      <c r="W17" s="1">
+        <v>6.62</v>
       </c>
       <c r="X17" s="1">
-        <v>104000000000</v>
-      </c>
-      <c r="Y17">
+        <v>5.23</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="Z17" s="1">
         <v>0</v>
       </c>
-      <c r="Z17">
-        <v>904000000</v>
-      </c>
-      <c r="AA17">
-        <v>58098000000</v>
-      </c>
-      <c r="AB17">
+      <c r="AA17" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>5.81</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>23.52</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>18.59</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>36.94</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>20.63</v>
+      </c>
+      <c r="AI17">
         <v>46.9</v>
       </c>
-      <c r="AC17">
+      <c r="AJ17">
         <v>63400000</v>
       </c>
-      <c r="AD17">
+      <c r="AK17">
         <v>155</v>
       </c>
-      <c r="AE17">
+      <c r="AL17">
         <v>2.5</v>
       </c>
-      <c r="AF17">
+      <c r="AM17">
         <v>86</v>
       </c>
-      <c r="AG17">
+      <c r="AN17">
         <v>2.27</v>
       </c>
-      <c r="AH17">
+      <c r="AO17">
         <v>613000</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>16754962</v>
       </c>
       <c r="E18">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="F18">
         <v>0.51</v>
@@ -2972,10 +3351,10 @@
         <v>33700</v>
       </c>
       <c r="L18" s="1">
-        <v>770000000000</v>
-      </c>
-      <c r="M18">
-        <v>45961</v>
+        <v>0.77</v>
+      </c>
+      <c r="M18" s="2">
+        <v>46</v>
       </c>
       <c r="N18">
         <v>1.53</v>
@@ -2984,13 +3363,13 @@
         <v>168</v>
       </c>
       <c r="P18" s="1">
-        <v>2660000000000</v>
-      </c>
-      <c r="Q18">
-        <v>226503</v>
-      </c>
-      <c r="R18">
-        <v>344</v>
+        <v>2.66</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>226.5</v>
+      </c>
+      <c r="R18" s="2">
+        <v>345.5</v>
       </c>
       <c r="S18">
         <v>6654000</v>
@@ -2998,64 +3377,85 @@
       <c r="T18">
         <v>39.799999999999997</v>
       </c>
-      <c r="U18" s="1">
-        <v>113000000000</v>
-      </c>
-      <c r="V18">
-        <v>24736000000</v>
-      </c>
-      <c r="W18">
-        <v>57000000</v>
-      </c>
-      <c r="X18">
-        <v>68438000000</v>
-      </c>
-      <c r="Y18">
-        <v>4141000000</v>
-      </c>
-      <c r="Z18">
-        <v>1454000000</v>
-      </c>
-      <c r="AA18">
-        <v>12318000000</v>
-      </c>
-      <c r="AB18">
+      <c r="U18">
+        <v>0.66</v>
+      </c>
+      <c r="V18" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="W18" s="1">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="X18" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>6.84</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>22.26</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>61.58</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>3.73</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>11.08</v>
+      </c>
+      <c r="AI18">
         <v>331</v>
       </c>
-      <c r="AC18">
+      <c r="AJ18">
         <v>31700000</v>
       </c>
-      <c r="AD18">
+      <c r="AK18">
         <v>527</v>
       </c>
-      <c r="AE18">
+      <c r="AL18">
         <v>4.2</v>
       </c>
-      <c r="AF18">
+      <c r="AM18">
         <v>115</v>
       </c>
-      <c r="AG18">
+      <c r="AN18">
         <v>0.48</v>
       </c>
-      <c r="AH18">
+      <c r="AO18">
         <v>43300</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>7996861</v>
       </c>
       <c r="E19">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F19">
         <v>1.04</v>
@@ -3076,10 +3476,10 @@
         <v>40000</v>
       </c>
       <c r="L19" s="1">
-        <v>631000000000</v>
-      </c>
-      <c r="M19">
-        <v>78929</v>
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="M19" s="2">
+        <v>78.900000000000006</v>
       </c>
       <c r="N19">
         <v>2.95</v>
@@ -3088,13 +3488,13 @@
         <v>94</v>
       </c>
       <c r="P19" s="1">
-        <v>1560000000000</v>
-      </c>
-      <c r="Q19">
-        <v>154063</v>
-      </c>
-      <c r="R19">
-        <v>229</v>
+        <v>1.56</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>154.1</v>
+      </c>
+      <c r="R19" s="2">
+        <v>247.2</v>
       </c>
       <c r="S19">
         <v>3210631</v>
@@ -3103,57 +3503,78 @@
         <v>40.1</v>
       </c>
       <c r="U19">
-        <v>62897000000</v>
-      </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
-      <c r="W19">
-        <v>32390000000</v>
-      </c>
-      <c r="X19">
-        <v>993000000</v>
-      </c>
-      <c r="Y19">
-        <v>26710000000</v>
-      </c>
-      <c r="Z19">
-        <v>58000000</v>
-      </c>
-      <c r="AA19">
-        <v>33998000000</v>
-      </c>
-      <c r="AB19">
+        <v>1.18</v>
+      </c>
+      <c r="V19" s="2">
+        <v>9.4</v>
+      </c>
+      <c r="W19" s="1">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>2.67</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>34.4</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>28.37</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>36.11</v>
+      </c>
+      <c r="AI19">
         <v>173</v>
       </c>
-      <c r="AC19">
+      <c r="AJ19">
         <v>26400000</v>
       </c>
-      <c r="AD19">
+      <c r="AK19">
         <v>566</v>
       </c>
-      <c r="AE19">
+      <c r="AL19">
         <v>5</v>
       </c>
-      <c r="AF19">
+      <c r="AM19">
         <v>123</v>
       </c>
-      <c r="AG19">
+      <c r="AN19">
         <v>0.49</v>
       </c>
-      <c r="AH19">
+      <c r="AO19">
         <v>22700</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>41086927</v>
@@ -3180,10 +3601,10 @@
         <v>2740000</v>
       </c>
       <c r="L20" s="1">
-        <v>603000000000</v>
-      </c>
-      <c r="M20">
-        <v>14680</v>
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="M20" s="2">
+        <v>14.7</v>
       </c>
       <c r="N20">
         <v>9.14</v>
@@ -3192,13 +3613,13 @@
         <v>30</v>
       </c>
       <c r="P20" s="1">
-        <v>334000000000</v>
-      </c>
-      <c r="Q20">
-        <v>7759</v>
-      </c>
-      <c r="R20">
-        <v>44.8</v>
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="R20" s="2">
+        <v>55.4</v>
       </c>
       <c r="S20">
         <v>5147626</v>
@@ -3206,58 +3627,79 @@
       <c r="T20">
         <v>12.5</v>
       </c>
-      <c r="U20" s="1">
-        <v>130000000000</v>
-      </c>
-      <c r="V20">
-        <v>3238000000</v>
-      </c>
-      <c r="W20">
-        <v>31564000000</v>
-      </c>
-      <c r="X20">
-        <v>66638000000</v>
-      </c>
-      <c r="Y20">
-        <v>6371000000</v>
-      </c>
-      <c r="Z20">
-        <v>19591000000</v>
-      </c>
-      <c r="AA20">
-        <v>33717000000</v>
-      </c>
-      <c r="AB20">
+      <c r="U20">
+        <v>0.39</v>
+      </c>
+      <c r="V20" s="2">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="W20" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="X20" s="1">
+        <v>3.16</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>6.66</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>1.96</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>3.37</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>19.59</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>41.36</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>12.16</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>20.93</v>
+      </c>
+      <c r="AI20">
         <v>15</v>
       </c>
-      <c r="AC20">
+      <c r="AJ20">
         <v>9380000</v>
       </c>
-      <c r="AD20">
+      <c r="AK20">
         <v>257</v>
       </c>
-      <c r="AE20">
+      <c r="AL20">
         <v>4.5</v>
       </c>
-      <c r="AF20">
+      <c r="AM20">
         <v>141</v>
       </c>
-      <c r="AG20">
+      <c r="AN20">
         <v>0.55000000000000004</v>
       </c>
-      <c r="AH20">
+      <c r="AO20">
         <v>104000</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>9519374</v>
@@ -3284,10 +3726,10 @@
         <v>410000</v>
       </c>
       <c r="L21" s="1">
-        <v>524000000000</v>
-      </c>
-      <c r="M21">
-        <v>55039</v>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="M21" s="2">
+        <v>55</v>
       </c>
       <c r="N21">
         <v>6.56</v>
@@ -3296,13 +3738,13 @@
         <v>91</v>
       </c>
       <c r="P21" s="1">
-        <v>1030000000000</v>
-      </c>
-      <c r="Q21">
-        <v>91487</v>
-      </c>
-      <c r="R21">
-        <v>187</v>
+        <v>1.03</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>91.5</v>
+      </c>
+      <c r="R21" s="2">
+        <v>196.6</v>
       </c>
       <c r="S21">
         <v>3069880</v>
@@ -3310,64 +3752,85 @@
       <c r="T21">
         <v>32.299999999999997</v>
       </c>
-      <c r="U21" s="1">
-        <v>150000000000</v>
-      </c>
-      <c r="V21">
-        <v>1391000000</v>
-      </c>
-      <c r="W21">
-        <v>66434000000</v>
-      </c>
-      <c r="X21">
-        <v>1549000000</v>
-      </c>
-      <c r="Y21">
-        <v>60475000000</v>
-      </c>
-      <c r="Z21">
-        <v>791000000</v>
-      </c>
-      <c r="AA21">
-        <v>84059000000</v>
-      </c>
-      <c r="AB21">
+      <c r="U21">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="V21" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="W21" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X21" s="1">
+        <v>6.64</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>8.41</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>30.94</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>28.17</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>39.15</v>
+      </c>
+      <c r="AI21">
         <v>128</v>
       </c>
-      <c r="AC21">
+      <c r="AJ21">
         <v>700000</v>
       </c>
-      <c r="AD21">
+      <c r="AK21">
         <v>520</v>
       </c>
-      <c r="AE21">
+      <c r="AL21">
         <v>2.7</v>
       </c>
-      <c r="AF21">
+      <c r="AM21">
         <v>117</v>
       </c>
-      <c r="AG21">
+      <c r="AN21">
         <v>0.32</v>
       </c>
-      <c r="AH21">
+      <c r="AO21">
         <v>16100</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>5018573</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22">
         <v>1.25</v>
@@ -3388,10 +3851,10 @@
         <v>304000</v>
       </c>
       <c r="L22" s="1">
-        <v>500000000000</v>
-      </c>
-      <c r="M22">
-        <v>99636</v>
+        <v>0.5</v>
+      </c>
+      <c r="M22" s="2">
+        <v>99.6</v>
       </c>
       <c r="N22">
         <v>0.48</v>
@@ -3400,13 +3863,13 @@
         <v>69</v>
       </c>
       <c r="P22" s="1">
-        <v>645000000000</v>
-      </c>
-      <c r="Q22">
-        <v>131220</v>
-      </c>
-      <c r="R22">
-        <v>141</v>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>131.19999999999999</v>
+      </c>
+      <c r="R22" s="2">
+        <v>129</v>
       </c>
       <c r="S22">
         <v>1814144</v>
@@ -3414,64 +3877,85 @@
       <c r="T22">
         <v>36.299999999999997</v>
       </c>
-      <c r="U22" s="1">
-        <v>127000000000</v>
-      </c>
-      <c r="V22">
-        <v>119000000</v>
+      <c r="U22">
+        <v>4.93</v>
+      </c>
+      <c r="V22" s="2">
+        <v>24.7</v>
       </c>
       <c r="W22" s="1">
-        <v>121000000000</v>
-      </c>
-      <c r="X22">
-        <v>4059000000</v>
+        <v>0.01</v>
+      </c>
+      <c r="X22" s="1">
+        <v>12.1</v>
       </c>
       <c r="Y22" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="Z22" s="1">
         <v>0</v>
       </c>
-      <c r="Z22">
-        <v>30000000</v>
-      </c>
       <c r="AA22" s="1">
-        <v>122000000000</v>
-      </c>
-      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>48.95</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>1.64</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>49.35</v>
+      </c>
+      <c r="AI22">
         <v>28.9</v>
       </c>
-      <c r="AC22">
+      <c r="AJ22">
         <v>400000</v>
       </c>
-      <c r="AD22">
+      <c r="AK22">
         <v>584</v>
       </c>
-      <c r="AE22">
+      <c r="AL22">
         <v>3.3</v>
       </c>
-      <c r="AF22">
+      <c r="AM22">
         <v>114</v>
       </c>
-      <c r="AG22">
+      <c r="AN22">
         <v>0.97</v>
       </c>
-      <c r="AH22">
+      <c r="AO22">
         <v>25800</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <v>38535873</v>
       </c>
       <c r="E23">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F23">
         <v>0.08</v>
@@ -3492,10 +3976,10 @@
         <v>304000</v>
       </c>
       <c r="L23" s="1">
-        <v>490000000000</v>
-      </c>
-      <c r="M23">
-        <v>12721</v>
+        <v>0.49</v>
+      </c>
+      <c r="M23" s="2">
+        <v>12.7</v>
       </c>
       <c r="N23">
         <v>3.88</v>
@@ -3504,13 +3988,13 @@
         <v>93</v>
       </c>
       <c r="P23" s="1">
-        <v>326000000000</v>
-      </c>
-      <c r="Q23">
-        <v>6586</v>
-      </c>
-      <c r="R23">
-        <v>47</v>
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="R23" s="2">
+        <v>66.5</v>
       </c>
       <c r="S23">
         <v>5954666</v>
@@ -3518,64 +4002,85 @@
       <c r="T23">
         <v>15.6</v>
       </c>
-      <c r="U23" s="1">
-        <v>163000000000</v>
-      </c>
-      <c r="V23" s="1">
-        <v>141000000000</v>
-      </c>
-      <c r="W23">
-        <v>2331000000</v>
-      </c>
-      <c r="X23">
-        <v>5821000000</v>
-      </c>
-      <c r="Y23">
+      <c r="U23">
+        <v>0.43</v>
+      </c>
+      <c r="V23" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="W23" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="X23" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Z23" s="1">
         <v>0</v>
       </c>
-      <c r="Z23">
-        <v>2453000000</v>
-      </c>
-      <c r="AA23">
-        <v>13138000000</v>
-      </c>
-      <c r="AB23">
+      <c r="AA23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>85.59</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="AE23" s="1">
+        <v>3.53</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>7.97</v>
+      </c>
+      <c r="AI23">
         <v>130</v>
       </c>
-      <c r="AC23">
+      <c r="AJ23">
         <v>4910000</v>
       </c>
-      <c r="AD23">
+      <c r="AK23">
         <v>532</v>
       </c>
-      <c r="AE23">
+      <c r="AL23">
         <v>6.5</v>
       </c>
-      <c r="AF23">
+      <c r="AM23">
         <v>123</v>
       </c>
-      <c r="AG23">
+      <c r="AN23">
         <v>0.93</v>
       </c>
-      <c r="AH23">
+      <c r="AO23">
         <v>173000</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <v>11128246</v>
       </c>
       <c r="E24">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="F24">
         <v>1.1399999999999999</v>
@@ -3596,10 +4101,10 @@
         <v>30300</v>
       </c>
       <c r="L24" s="1">
-        <v>483000000000</v>
-      </c>
-      <c r="M24">
-        <v>43396</v>
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="M24" s="2">
+        <v>43.4</v>
       </c>
       <c r="N24">
         <v>2.34</v>
@@ -3608,13 +4113,13 @@
         <v>171</v>
       </c>
       <c r="P24" s="1">
-        <v>1420000000000</v>
-      </c>
-      <c r="Q24">
-        <v>113603</v>
-      </c>
-      <c r="R24">
-        <v>266</v>
+        <v>1.42</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>113.6</v>
+      </c>
+      <c r="R24" s="2">
+        <v>294</v>
       </c>
       <c r="S24">
         <v>3679196</v>
@@ -3623,57 +4128,78 @@
         <v>33.299999999999997</v>
       </c>
       <c r="U24">
-        <v>89008000000</v>
-      </c>
-      <c r="V24">
-        <v>5375000000</v>
-      </c>
-      <c r="W24">
-        <v>196000000</v>
-      </c>
-      <c r="X24">
-        <v>25438000000</v>
-      </c>
-      <c r="Y24">
-        <v>48234000000</v>
-      </c>
-      <c r="Z24">
-        <v>290000000</v>
-      </c>
-      <c r="AA24">
-        <v>8377000000</v>
-      </c>
-      <c r="AB24">
+        <v>0.79</v>
+      </c>
+      <c r="V24" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="W24" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="X24" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>2.54</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="AE24" s="1">
+        <v>28.94</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>54.87</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="AI24">
         <v>504</v>
       </c>
-      <c r="AC24">
+      <c r="AJ24">
         <v>9510000</v>
       </c>
-      <c r="AD24">
+      <c r="AK24">
         <v>559</v>
       </c>
-      <c r="AE24">
+      <c r="AL24">
         <v>6.53</v>
       </c>
-      <c r="AF24">
+      <c r="AM24">
         <v>111</v>
       </c>
-      <c r="AG24">
+      <c r="AN24">
         <v>0.63</v>
       </c>
-      <c r="AH24">
+      <c r="AO24">
         <v>30700</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <v>8429991</v>
@@ -3700,10 +4226,10 @@
         <v>82400</v>
       </c>
       <c r="L25" s="1">
-        <v>394000000000</v>
-      </c>
-      <c r="M25">
-        <v>46792</v>
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="M25" s="2">
+        <v>46.7</v>
       </c>
       <c r="N25">
         <v>1.77</v>
@@ -3712,13 +4238,13 @@
         <v>111</v>
       </c>
       <c r="P25" s="1">
-        <v>884000000000</v>
-      </c>
-      <c r="Q25">
-        <v>90128</v>
-      </c>
-      <c r="R25">
-        <v>200</v>
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>90.1</v>
+      </c>
+      <c r="R25" s="2">
+        <v>224.4</v>
       </c>
       <c r="S25">
         <v>2118000</v>
@@ -3727,49 +4253,71 @@
         <v>25</v>
       </c>
       <c r="U25">
-        <v>62160000000</v>
-      </c>
-      <c r="V25">
-        <v>7321000000</v>
-      </c>
-      <c r="W25">
-        <v>34180000000</v>
-      </c>
-      <c r="X25">
-        <v>12394000000</v>
-      </c>
-      <c r="Y25">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="V25" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="X25" s="1">
+        <v>3.42</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="Z25" s="1">
         <v>0</v>
       </c>
-      <c r="Z25">
-        <v>1011000000</v>
-      </c>
-      <c r="AA25">
-        <v>40815000000</v>
-      </c>
-      <c r="AB25">
+      <c r="AA25" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>4.08</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>7.65</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>35.71</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>12.95</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="AH25" s="1">
+        <v>42.64</v>
+      </c>
+      <c r="AI25">
         <v>131</v>
       </c>
-      <c r="AC25">
+      <c r="AJ25">
         <v>14500000</v>
       </c>
-      <c r="AD25">
+      <c r="AK25">
         <v>578</v>
       </c>
-      <c r="AE25">
+      <c r="AL25">
         <v>7.6</v>
       </c>
-      <c r="AF25">
+      <c r="AM25">
         <v>146</v>
       </c>
-      <c r="AG25">
+      <c r="AN25">
         <v>0.52</v>
       </c>
-      <c r="AH25">
+      <c r="AO25">
         <v>22800</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>